<commit_message>
update to axes, in excel
</commit_message>
<xml_diff>
--- a/Aufgabe10/Messungen.xlsx
+++ b/Aufgabe10/Messungen.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dima\Documents\sablony\Aufgabe10\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="11715" windowHeight="7740"/>
   </bookViews>
@@ -54,8 +59,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,12 +246,6 @@
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -256,14 +255,20 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -280,7 +285,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="de-DE"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -300,11 +315,14 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -385,6 +403,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -466,6 +485,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -523,17 +543,70 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$3:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="73202304"/>
-        <c:axId val="74723712"/>
+        <c:smooth val="0"/>
+        <c:axId val="443613416"/>
+        <c:axId val="443617336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73202304"/>
+        <c:axId val="443613416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -552,9 +625,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -586,23 +661,24 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74723712"/>
+        <c:crossAx val="443617336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74723712"/>
+        <c:axId val="443617336"/>
         <c:scaling>
-          <c:logBase val="9"/>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="150000000"/>
-          <c:min val="200000"/>
+          <c:min val="100000"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
@@ -620,6 +696,7 @@
         </c:majorGridlines>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -645,12 +722,13 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73202304"/>
+        <c:crossAx val="443613416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:minorUnit val="10"/>
         <c:dispUnits>
           <c:builtInUnit val="thousands"/>
           <c:dispUnitsLbl>
@@ -685,6 +763,7 @@
     <c:legend>
       <c:legendPos val="t"/>
       <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -709,12 +788,13 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -738,7 +818,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -755,12 +835,12 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>60325</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>10052</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>116417</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>226483</xdr:colOff>
+      <xdr:colOff>306917</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>52915</xdr:rowOff>
     </xdr:to>
@@ -785,9 +865,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -825,9 +905,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -859,9 +939,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -893,9 +974,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1068,121 +1150,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="13" style="5" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="13" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="5"/>
+    <col min="1" max="1" width="20.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="13" style="3" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="13" style="3" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="13"/>
-      <c r="D1" s="3"/>
-      <c r="F1" s="14" t="s">
+      <c r="D1" s="14"/>
+      <c r="F1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="9">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>10000</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
         <v>2197905</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>232991</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>5193399</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="9">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>100000</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
         <v>8494865</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>326369</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="8">
         <v>15622660</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="9">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>1000000</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <v>17028003</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>364571</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <v>33580249</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="11">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
         <v>10000000</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="9">
         <v>123726759</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="10">
         <v>1569124</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="10">
         <v>213990449</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1197,24 +1279,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>